<commit_message>
added more analysis for eLife revisions
</commit_message>
<xml_diff>
--- a/USA/state/write_ups/01_wavelet_paper/tables/Table 2 2018 06 19.xlsx
+++ b/USA/state/write_ups/01_wavelet_paper/tables/Table 2 2018 06 19.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-3360" yWindow="-19780" windowWidth="18080" windowHeight="18220" tabRatio="500"/>
+    <workbookView xWindow="-3340" yWindow="-19780" windowWidth="29840" windowHeight="18220" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Climate region</t>
   </si>
@@ -32,9 +32,6 @@
     <t>Population (2016)</t>
   </si>
   <si>
-    <t>Percentage of land mass of contiguous USA</t>
-  </si>
-  <si>
     <t>Poverty rates etc?</t>
   </si>
   <si>
@@ -66,12 +63,48 @@
   </si>
   <si>
     <t>Mean annual temperature (1980-2016) (°C)</t>
+  </si>
+  <si>
+    <t>Illinois, Indiana, Kentucky, Missouri, Ohio, Tennessee, West Virginia</t>
+  </si>
+  <si>
+    <t>Iowa, Michigan, Minnesota, Wisconsin</t>
+  </si>
+  <si>
+    <t>Connecticut, Delaware, Maine, Maryland, Massachusetts, New Hampshire, New Jersey, New York, Pennsylvania, Rhode Island, Vermont</t>
+  </si>
+  <si>
+    <t>Arkansas, Kansas, Louisiana, Mississippi, Oklahoma, Texas</t>
+  </si>
+  <si>
+    <t>Alabama, Florida, Georgia, North Carolina, South Carolina, Virginia</t>
+  </si>
+  <si>
+    <t>Arizona, Colorado, New Mexico, Utah</t>
+  </si>
+  <si>
+    <t>Montana, Nebraska, North Dakota, South Dakota, Wyoming</t>
+  </si>
+  <si>
+    <t>Constituent states</t>
+  </si>
+  <si>
+    <t>Alaska, Idaho, Oregon, Washington</t>
+  </si>
+  <si>
+    <t>California, Hawaii, Nevada</t>
+  </si>
+  <si>
+    <t>Percentage of land mass of USA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000000"/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -136,7 +169,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -144,8 +177,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
@@ -156,14 +193,26 @@
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -439,169 +488,243 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.1640625" style="7" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.83203125" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="61" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="61" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:8" ht="46" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="C2" s="4">
+        <v>50191326</v>
+      </c>
+      <c r="D2" s="2">
+        <v>10.27</v>
+      </c>
+      <c r="E2" s="2">
+        <v>11.6</v>
+      </c>
+      <c r="F2" s="2"/>
+      <c r="H2" s="8">
+        <f>C2/$H$11</f>
+        <v>0.15505295758884766</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="4">
-        <v>50191326</v>
-      </c>
-      <c r="C2" s="2">
-        <v>10.27</v>
-      </c>
-      <c r="D2" s="2">
-        <v>11.6</v>
-      </c>
-      <c r="E2" s="2"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+      <c r="B3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="4">
+        <v>24418738</v>
+      </c>
+      <c r="D3" s="2">
+        <v>8.43</v>
+      </c>
+      <c r="E3" s="2">
+        <v>8</v>
+      </c>
+      <c r="F3" s="2"/>
+      <c r="H3" s="8">
+        <f>C3/$H$11</f>
+        <v>7.5435296279822997E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="80" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="4">
-        <v>24418738</v>
-      </c>
-      <c r="C3" s="2">
-        <v>8.43</v>
-      </c>
-      <c r="D3" s="2">
+      <c r="B4" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="4">
+        <v>64046741</v>
+      </c>
+      <c r="D4" s="2">
+        <v>6.02</v>
+      </c>
+      <c r="E4" s="2">
+        <v>10.6</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="H4" s="8">
+        <f>C4/$H$11</f>
+        <v>0.19785563377976728</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="4">
+        <v>13811810</v>
+      </c>
+      <c r="D5" s="2">
+        <v>8.23</v>
+      </c>
+      <c r="E5" s="2">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="F5" s="2"/>
+      <c r="H5" s="8">
+        <f>C5/$H$11</f>
+        <v>4.2667969962682836E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="4">
+        <v>45388414</v>
+      </c>
+      <c r="D6" s="2">
+        <v>18.82</v>
+      </c>
+      <c r="E6" s="2">
+        <v>18</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="H6" s="8">
+        <f>C6/$H$11</f>
+        <v>0.14021561874988239</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="4">
+        <v>59356072</v>
+      </c>
+      <c r="D7" s="2">
+        <v>9.7200000000000006</v>
+      </c>
+      <c r="E7" s="2">
+        <v>18.399999999999999</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="H7" s="8">
+        <f>C7/$H$11</f>
+        <v>0.18336504029514161</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="2"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4">
-        <v>64046741</v>
-      </c>
-      <c r="C4" s="2">
-        <v>6.02</v>
-      </c>
-      <c r="D4" s="2">
-        <v>10.6</v>
-      </c>
-      <c r="E4" s="2"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="4">
-        <v>13811810</v>
-      </c>
-      <c r="C5" s="2">
-        <v>8.23</v>
-      </c>
-      <c r="D5" s="2">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="E5" s="2"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="4">
-        <v>45388414</v>
-      </c>
-      <c r="C6" s="2">
-        <v>18.82</v>
-      </c>
-      <c r="D6" s="2">
+      <c r="B8" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="2"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="4">
-        <v>59356072</v>
-      </c>
-      <c r="C7" s="2">
-        <v>9.7200000000000006</v>
-      </c>
-      <c r="D7" s="2">
-        <v>18.399999999999999</v>
-      </c>
-      <c r="E7" s="2"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+      <c r="C8" s="4">
+        <v>17613981</v>
+      </c>
+      <c r="D8" s="2">
+        <v>14.05</v>
+      </c>
+      <c r="E8" s="2">
+        <v>13.6</v>
+      </c>
+      <c r="F8" s="2"/>
+      <c r="H8" s="8">
+        <f>C8/$H$11</f>
+        <v>5.441378155587618E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="4">
-        <v>17613981</v>
-      </c>
-      <c r="C8" s="2">
-        <v>14.05</v>
-      </c>
-      <c r="D8" s="2">
-        <v>13.6</v>
-      </c>
-      <c r="E8" s="2"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
+      <c r="B9" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="4">
+        <v>43708574</v>
+      </c>
+      <c r="D9" s="2">
+        <v>8.91</v>
+      </c>
+      <c r="E9" s="2">
+        <v>16.600000000000001</v>
+      </c>
+      <c r="F9" s="2"/>
+      <c r="H9" s="8">
+        <f>C9/$H$11</f>
+        <v>0.13502619298583604</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="4">
-        <v>43708574</v>
-      </c>
-      <c r="C9" s="2">
-        <v>8.91</v>
-      </c>
-      <c r="D9" s="2">
-        <v>16.600000000000001</v>
-      </c>
-      <c r="E9" s="2"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="4">
+      <c r="B10" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="4">
         <v>5168753</v>
       </c>
-      <c r="C10" s="2">
+      <c r="D10" s="2">
         <v>15.55</v>
       </c>
-      <c r="D10" s="2">
+      <c r="E10" s="2">
         <v>7.6</v>
       </c>
-      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="H10" s="8">
+        <f>C10/$H$11</f>
+        <v>1.5967508802143007E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H11" s="9">
+        <f>SUM(C2:C10)</f>
+        <v>323704409</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>